<commit_message>
Update Jeopardy Questions spreadsheet
</commit_message>
<xml_diff>
--- a/JeopardyQuestions.xlsx
+++ b/JeopardyQuestions.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="315" windowWidth="13980" windowHeight="11190"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,11 +14,15 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$129</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
   </pivotCaches>
-  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -2503,26 +2507,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:I129"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E44" sqref="E44"/>
+      <selection pane="bottomLeft" activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="9.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="57.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="19.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="5" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="57.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>152</v>
       </c>
@@ -2551,7 +2555,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="70" hidden="1">
       <c r="A2">
         <f>ROW()</f>
         <v>2</v>
@@ -2582,7 +2586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="70" hidden="1">
       <c r="A3">
         <f>ROW()</f>
         <v>3</v>
@@ -2607,7 +2611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="70" hidden="1">
       <c r="A4">
         <f>ROW()</f>
         <v>4</v>
@@ -2632,7 +2636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="70" hidden="1">
       <c r="A5">
         <f>ROW()</f>
         <v>5</v>
@@ -2657,7 +2661,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="70" hidden="1">
       <c r="A6">
         <f>ROW()</f>
         <v>6</v>
@@ -2682,7 +2686,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="70">
       <c r="A7">
         <f>ROW()</f>
         <v>7</v>
@@ -2707,7 +2711,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="70">
       <c r="A8">
         <f>ROW()</f>
         <v>8</v>
@@ -2732,7 +2736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="70" hidden="1">
       <c r="A9">
         <f>ROW()</f>
         <v>9</v>
@@ -2757,7 +2761,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="56" hidden="1">
       <c r="A10">
         <f>ROW()</f>
         <v>10</v>
@@ -2776,7 +2780,7 @@
         <v>&lt;div class="clue jbg" rel="#10"&gt;&lt;h2 class="value"&gt;10&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="10"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Corinth ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="70" hidden="1">
       <c r="A11">
         <f>ROW()</f>
         <v>11</v>
@@ -2798,7 +2802,7 @@
         <v>&lt;div class="clue jbg" rel="#11"&gt;&lt;h2 class="value"&gt;10&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="11"&gt; &lt;p class="prompt"&gt;the nation made up of descendants of the 12 tribes of Jacob&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Israel ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="56" hidden="1">
       <c r="A12">
         <f>ROW()</f>
         <v>12</v>
@@ -2817,7 +2821,7 @@
         <v>&lt;div class="clue jbg" rel="#12"&gt;&lt;h2 class="value"&gt;10&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="12"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is the Mount of Olives ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="70" hidden="1">
       <c r="A13">
         <f>ROW()</f>
         <v>13</v>
@@ -2848,7 +2852,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="70" hidden="1">
       <c r="A14">
         <f>ROW()</f>
         <v>14</v>
@@ -2870,7 +2874,7 @@
         <v>&lt;div class="clue jbg" rel="#14"&gt;&lt;h2 class="value"&gt;20&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="14"&gt; &lt;p class="prompt"&gt;this north flowing Egyptian river was turned to blood due to a plague&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is the Nile River ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="70" hidden="1">
       <c r="A15">
         <f>ROW()</f>
         <v>15</v>
@@ -2895,7 +2899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="70" hidden="1">
       <c r="A16">
         <f>ROW()</f>
         <v>16</v>
@@ -2920,7 +2924,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="70">
       <c r="A17">
         <f>ROW()</f>
         <v>17</v>
@@ -2951,7 +2955,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="70" hidden="1">
       <c r="A18">
         <f>ROW()</f>
         <v>18</v>
@@ -2976,7 +2980,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="70" hidden="1">
       <c r="A19">
         <f>ROW()</f>
         <v>19</v>
@@ -2992,7 +2996,7 @@
         <v>&lt;div class="clue jbg" rel="#19"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="19"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is the Great Sea (Mediterranean) ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="84">
       <c r="A20">
         <f>ROW()</f>
         <v>20</v>
@@ -3017,7 +3021,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="56" hidden="1">
       <c r="A21">
         <f>ROW()</f>
         <v>21</v>
@@ -3033,7 +3037,7 @@
         <v>&lt;div class="clue jbg" rel="#21"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="21"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Giza ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="56" hidden="1">
       <c r="A22">
         <f>ROW()</f>
         <v>22</v>
@@ -3049,7 +3053,7 @@
         <v>&lt;div class="clue jbg" rel="#22"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="22"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Rome ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="56" hidden="1">
       <c r="A23">
         <f>ROW()</f>
         <v>23</v>
@@ -3065,7 +3069,7 @@
         <v>&lt;div class="clue jbg" rel="#23"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="23"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Ephesus ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="56" hidden="1">
       <c r="A24">
         <f>ROW()</f>
         <v>24</v>
@@ -3081,7 +3085,7 @@
         <v>&lt;div class="clue jbg" rel="#24"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="24"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Casaerea Phillipi ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="56" hidden="1">
       <c r="A25">
         <f>ROW()</f>
         <v>25</v>
@@ -3097,7 +3101,7 @@
         <v>&lt;div class="clue jbg" rel="#25"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="25"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Sidon ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" ht="56" hidden="1">
       <c r="A26">
         <f>ROW()</f>
         <v>26</v>
@@ -3113,7 +3117,7 @@
         <v>&lt;div class="clue jbg" rel="#26"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="26"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Tyre ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="70">
       <c r="A27">
         <f>ROW()</f>
         <v>27</v>
@@ -3144,7 +3148,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="56" hidden="1">
       <c r="A28">
         <f>ROW()</f>
         <v>28</v>
@@ -3160,7 +3164,7 @@
         <v>&lt;div class="clue jbg" rel="#28"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="28"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Bethany ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="56" hidden="1">
       <c r="A29">
         <f>ROW()</f>
         <v>29</v>
@@ -3176,7 +3180,7 @@
         <v>&lt;div class="clue jbg" rel="#29"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="29"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Samaria ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="56" hidden="1">
       <c r="A30">
         <f>ROW()</f>
         <v>30</v>
@@ -3192,7 +3196,7 @@
         <v>&lt;div class="clue jbg" rel="#30"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="30"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Damascus ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="56" hidden="1">
       <c r="A31">
         <f>ROW()</f>
         <v>31</v>
@@ -3208,7 +3212,7 @@
         <v>&lt;div class="clue jbg" rel="#31"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="31"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Joppa ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="56" hidden="1">
       <c r="A32">
         <f>ROW()</f>
         <v>32</v>
@@ -3224,7 +3228,7 @@
         <v>&lt;div class="clue jbg" rel="#32"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="32"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Where is Mount Nebo ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="70" hidden="1">
       <c r="A33">
         <f>ROW()</f>
         <v>33</v>
@@ -3249,7 +3253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="70" hidden="1">
       <c r="A34">
         <f>ROW()</f>
         <v>34</v>
@@ -3274,7 +3278,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="70" hidden="1">
       <c r="A35">
         <f>ROW()</f>
         <v>35</v>
@@ -3299,7 +3303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="70" hidden="1">
       <c r="A36">
         <f>ROW()</f>
         <v>36</v>
@@ -3324,7 +3328,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="120" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="84" hidden="1">
       <c r="A37">
         <f>ROW()</f>
         <v>37</v>
@@ -3349,7 +3353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="70" hidden="1">
       <c r="A38">
         <f>ROW()</f>
         <v>38</v>
@@ -3380,7 +3384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="84" hidden="1">
       <c r="A39">
         <f>ROW()</f>
         <v>39</v>
@@ -3405,7 +3409,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="70" hidden="1">
       <c r="A40">
         <f>ROW()</f>
         <v>40</v>
@@ -3436,7 +3440,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="70" hidden="1">
       <c r="A41">
         <f>ROW()</f>
         <v>41</v>
@@ -3467,7 +3471,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="165" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="126" hidden="1">
       <c r="A42">
         <f>ROW()</f>
         <v>42</v>
@@ -3492,7 +3496,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="84">
       <c r="A43">
         <f>ROW()</f>
         <v>43</v>
@@ -3523,7 +3527,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="56">
       <c r="A44">
         <f>ROW()</f>
         <v>44</v>
@@ -3548,7 +3552,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="120" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="84">
       <c r="A45">
         <f>ROW()</f>
         <v>45</v>
@@ -3573,7 +3577,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="70">
       <c r="A46">
         <f>ROW()</f>
         <v>46</v>
@@ -3598,7 +3602,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" ht="70">
       <c r="A47">
         <f>ROW()</f>
         <v>47</v>
@@ -3629,7 +3633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="70" hidden="1">
       <c r="A48">
         <f>ROW()</f>
         <v>48</v>
@@ -3660,7 +3664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" ht="70" hidden="1">
       <c r="A49">
         <f>ROW()</f>
         <v>49</v>
@@ -3691,7 +3695,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" ht="70" hidden="1">
       <c r="A50">
         <f>ROW()</f>
         <v>50</v>
@@ -3722,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" ht="70" hidden="1">
       <c r="A51">
         <f>ROW()</f>
         <v>51</v>
@@ -3753,7 +3757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" ht="70" hidden="1">
       <c r="A52">
         <f>ROW()</f>
         <v>52</v>
@@ -3784,7 +3788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" ht="56" hidden="1">
       <c r="A53">
         <f>ROW()</f>
         <v>53</v>
@@ -3815,7 +3819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" ht="70" hidden="1">
       <c r="A54">
         <f>ROW()</f>
         <v>54</v>
@@ -3846,7 +3850,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" ht="70">
       <c r="A55">
         <f>ROW()</f>
         <v>55</v>
@@ -3877,7 +3881,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" ht="70" hidden="1">
       <c r="A56">
         <f>ROW()</f>
         <v>56</v>
@@ -3908,7 +3912,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" ht="70" hidden="1">
       <c r="A57">
         <f>ROW()</f>
         <v>57</v>
@@ -3939,7 +3943,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" ht="84" hidden="1">
       <c r="A58">
         <f>ROW()</f>
         <v>58</v>
@@ -3970,7 +3974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" ht="70">
       <c r="A59">
         <f>ROW()</f>
         <v>59</v>
@@ -4001,7 +4005,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" ht="70">
       <c r="A60">
         <f>ROW()</f>
         <v>60</v>
@@ -4032,7 +4036,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" ht="70">
       <c r="A61">
         <f>ROW()</f>
         <v>61</v>
@@ -4063,7 +4067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="70">
       <c r="A62">
         <f>ROW()</f>
         <v>62</v>
@@ -4094,7 +4098,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" ht="70" hidden="1">
       <c r="A63">
         <f>ROW()</f>
         <v>63</v>
@@ -4125,7 +4129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" ht="70" hidden="1">
       <c r="A64">
         <f>ROW()</f>
         <v>64</v>
@@ -4156,7 +4160,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" ht="70" hidden="1">
       <c r="A65">
         <f>ROW()</f>
         <v>65</v>
@@ -4187,7 +4191,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" ht="84" hidden="1">
       <c r="A66">
         <f>ROW()</f>
         <v>66</v>
@@ -4218,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" ht="70" hidden="1">
       <c r="A67">
         <f>ROW()</f>
         <v>67</v>
@@ -4249,7 +4253,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" ht="84" hidden="1">
       <c r="A68">
         <f>ROW()</f>
         <v>68</v>
@@ -4280,7 +4284,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" ht="70" hidden="1">
       <c r="A69">
         <f>ROW()</f>
         <v>69</v>
@@ -4311,7 +4315,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" ht="70">
       <c r="A70">
         <f>ROW()</f>
         <v>70</v>
@@ -4342,7 +4346,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="150" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" ht="126" hidden="1">
       <c r="A71">
         <f>ROW()</f>
         <v>71</v>
@@ -4373,7 +4377,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" ht="70" hidden="1">
       <c r="A72">
         <f>ROW()</f>
         <v>72</v>
@@ -4404,7 +4408,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" ht="70" hidden="1">
       <c r="A73">
         <f>ROW()</f>
         <v>73</v>
@@ -4435,7 +4439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" ht="70">
       <c r="A74">
         <f>ROW()</f>
         <v>74</v>
@@ -4466,7 +4470,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="75" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" ht="70">
       <c r="A75">
         <f>ROW()</f>
         <v>75</v>
@@ -4497,7 +4501,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" ht="56" hidden="1">
       <c r="A76">
         <f>ROW()</f>
         <v>76</v>
@@ -4528,7 +4532,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" ht="70" hidden="1">
       <c r="A77">
         <f>ROW()</f>
         <v>77</v>
@@ -4559,7 +4563,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" ht="70" hidden="1">
       <c r="A78">
         <f>ROW()</f>
         <v>78</v>
@@ -4590,7 +4594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" ht="70" hidden="1">
       <c r="A79">
         <f>ROW()</f>
         <v>79</v>
@@ -4621,7 +4625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" ht="84" hidden="1">
       <c r="A80">
         <f>ROW()</f>
         <v>80</v>
@@ -4649,7 +4653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" ht="70" hidden="1">
       <c r="A81">
         <f>ROW()</f>
         <v>81</v>
@@ -4677,7 +4681,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" ht="84" hidden="1">
       <c r="A82">
         <f>ROW()</f>
         <v>82</v>
@@ -4708,7 +4712,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" ht="70" hidden="1">
       <c r="A83">
         <f>ROW()</f>
         <v>83</v>
@@ -4739,7 +4743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" ht="84" hidden="1">
       <c r="A84">
         <f>ROW()</f>
         <v>84</v>
@@ -4770,7 +4774,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" ht="70" hidden="1">
       <c r="A85">
         <f>ROW()</f>
         <v>85</v>
@@ -4801,7 +4805,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" ht="84">
       <c r="A86">
         <f>ROW()</f>
         <v>86</v>
@@ -4832,7 +4836,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="87" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" ht="70">
       <c r="A87">
         <f>ROW()</f>
         <v>87</v>
@@ -4863,7 +4867,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" ht="70">
       <c r="A88">
         <f>ROW()</f>
         <v>88</v>
@@ -4894,7 +4898,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="89" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" ht="84">
       <c r="A89">
         <f>ROW()</f>
         <v>89</v>
@@ -4925,7 +4929,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" ht="70">
       <c r="A90">
         <f>ROW()</f>
         <v>90</v>
@@ -4956,7 +4960,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="91" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" ht="70" hidden="1">
       <c r="A91">
         <f>ROW()</f>
         <v>91</v>
@@ -4978,7 +4982,7 @@
         <v>&lt;div class="clue jbg" rel="#91"&gt;&lt;h2 class="value"&gt;?&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="91"&gt; &lt;p class="prompt"&gt;List the time(s) the Jordan River was parted and by who&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is by Joshua, by Elijah, and by Elisha ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="92" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" ht="70" hidden="1">
       <c r="A92">
         <f>ROW()</f>
         <v>92</v>
@@ -5009,7 +5013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" ht="70" hidden="1">
       <c r="A93">
         <f>ROW()</f>
         <v>93</v>
@@ -5040,7 +5044,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" ht="70" hidden="1">
       <c r="A94">
         <f>ROW()</f>
         <v>94</v>
@@ -5065,7 +5069,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" ht="70" hidden="1">
       <c r="A95">
         <f>ROW()</f>
         <v>95</v>
@@ -5090,7 +5094,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" ht="70" hidden="1">
       <c r="A96">
         <f>ROW()</f>
         <v>96</v>
@@ -5115,7 +5119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" ht="84" hidden="1">
       <c r="A97">
         <f>ROW()</f>
         <v>97</v>
@@ -5140,7 +5144,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" ht="70" hidden="1">
       <c r="A98">
         <f>ROW()</f>
         <v>98</v>
@@ -5171,7 +5175,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" ht="70" hidden="1">
       <c r="A99">
         <f>ROW()</f>
         <v>99</v>
@@ -5196,7 +5200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:9" ht="93" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" ht="93" hidden="1" customHeight="1">
       <c r="A100">
         <f>ROW()</f>
         <v>100</v>
@@ -5221,7 +5225,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="101" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" ht="70" hidden="1">
       <c r="A101">
         <f>ROW()</f>
         <v>101</v>
@@ -5246,7 +5250,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" ht="70">
       <c r="A102">
         <f>ROW()</f>
         <v>102</v>
@@ -5277,7 +5281,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="103" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" ht="84">
       <c r="A103">
         <f>ROW()</f>
         <v>103</v>
@@ -5308,7 +5312,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" ht="84">
       <c r="A104">
         <f>ROW()</f>
         <v>104</v>
@@ -5333,7 +5337,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="105" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" ht="84">
       <c r="A105">
         <f>ROW()</f>
         <v>105</v>
@@ -5358,7 +5362,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="106" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" ht="70">
       <c r="A106">
         <f>ROW()</f>
         <v>106</v>
@@ -5389,7 +5393,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="107" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" ht="70" hidden="1">
       <c r="A107">
         <f>ROW()</f>
         <v>107</v>
@@ -5411,7 +5415,7 @@
         <v>&lt;div class="clue jbg" rel="#107"&gt;&lt;h2 class="value"&gt;10&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="107"&gt; &lt;p class="prompt"&gt;the intimate and personal name of God; it emphasizes his role as Israel's Redeemer and master&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is the Lord ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" ht="56" hidden="1">
       <c r="A108">
         <f>ROW()</f>
         <v>108</v>
@@ -5433,7 +5437,7 @@
         <v>&lt;div class="clue jbg" rel="#108"&gt;&lt;h2 class="value"&gt;10&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="108"&gt; &lt;p class="prompt"&gt;ruler over a country or kingdom&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Who is a king ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="109" spans="1:9" ht="105" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" ht="84" hidden="1">
       <c r="A109">
         <f>ROW()</f>
         <v>109</v>
@@ -5455,7 +5459,7 @@
         <v>&lt;div class="clue jbg" rel="#109"&gt;&lt;h2 class="value"&gt;10&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="109"&gt; &lt;p class="prompt"&gt;someone who takes care of a flock of sheep. This word is often used in the Bible as a figure of speech for anyone who cares for a group of people.&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;Who is a shepherd ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" ht="70" hidden="1">
       <c r="A110">
         <f>ROW()</f>
         <v>110</v>
@@ -5477,7 +5481,7 @@
         <v>&lt;div class="clue jbg" rel="#110"&gt;&lt;h2 class="value"&gt;20&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="110"&gt; &lt;p class="prompt"&gt;a book made of a long piece of leather or paper that was rolled around a stick at both ends&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;what is a scroll ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" ht="56" hidden="1">
       <c r="A111">
         <f>ROW()</f>
         <v>111</v>
@@ -5499,7 +5503,7 @@
         <v>&lt;div class="clue jbg" rel="#111"&gt;&lt;h2 class="value"&gt;20&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="111"&gt; &lt;p class="prompt"&gt;the part of a person that is not the body&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is a spirit ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="112" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" ht="70" hidden="1">
       <c r="A112">
         <f>ROW()</f>
         <v>112</v>
@@ -5521,7 +5525,7 @@
         <v>&lt;div class="clue jbg" rel="#112"&gt;&lt;h2 class="value"&gt;20&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="112"&gt; &lt;p class="prompt"&gt;goodwill; a positive attitude toward another person&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is favor ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="113" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" ht="70" hidden="1">
       <c r="A113">
         <f>ROW()</f>
         <v>113</v>
@@ -5543,7 +5547,7 @@
         <v>&lt;div class="clue jbg" rel="#113"&gt;&lt;h2 class="value"&gt;20&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="113"&gt; &lt;p class="prompt"&gt;telling the message of the gospel in public; delivering a sermon&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is preaching ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="114" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" ht="56" hidden="1">
       <c r="A114">
         <f>ROW()</f>
         <v>114</v>
@@ -5565,7 +5569,7 @@
         <v>&lt;div class="clue jbg" rel="#114"&gt;&lt;h2 class="value"&gt;20&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="114"&gt; &lt;p class="prompt"&gt;a binding promise or agreement&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is a pledge ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" ht="70" hidden="1">
       <c r="A115">
         <f>ROW()</f>
         <v>115</v>
@@ -5587,7 +5591,7 @@
         <v>&lt;div class="clue jbg" rel="#115"&gt;&lt;h2 class="value"&gt;20&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="115"&gt; &lt;p class="prompt"&gt;honor; praise; a source of pride or worthiness&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is glory ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="116" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" ht="56" hidden="1">
       <c r="A116">
         <f>ROW()</f>
         <v>116</v>
@@ -5609,7 +5613,7 @@
         <v>&lt;div class="clue jbg" rel="#116"&gt;&lt;h2 class="value"&gt;20&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="116"&gt; &lt;p class="prompt"&gt;firm belief or faith in another&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is trust ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="117" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" ht="56" hidden="1">
       <c r="A117">
         <f>ROW()</f>
         <v>117</v>
@@ -5631,7 +5635,7 @@
         <v>&lt;div class="clue jbg" rel="#117"&gt;&lt;h2 class="value"&gt;30&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="117"&gt; &lt;p class="prompt"&gt;a wise saying&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is a proverb ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="118" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" ht="84" hidden="1">
       <c r="A118">
         <f>ROW()</f>
         <v>118</v>
@@ -5653,7 +5657,7 @@
         <v>&lt;div class="clue jbg" rel="#118"&gt;&lt;h2 class="value"&gt;30&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="118"&gt; &lt;p class="prompt"&gt;one who cares after your physical well-being, typicall experienced in medicine. Luke was this.&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is a physician ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="119" spans="1:9" ht="90" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" ht="70" hidden="1">
       <c r="A119">
         <f>ROW()</f>
         <v>119</v>
@@ -5675,7 +5679,7 @@
         <v>&lt;div class="clue jbg" rel="#119"&gt;&lt;h2 class="value"&gt;30&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="119"&gt; &lt;p class="prompt"&gt;a time when there is not enough food or any severe shortage&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is a famine ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="120" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" ht="56" hidden="1">
       <c r="A120">
         <f>ROW()</f>
         <v>120</v>
@@ -5697,7 +5701,7 @@
         <v>&lt;div class="clue jbg" rel="#120"&gt;&lt;h2 class="value"&gt;30&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="120"&gt; &lt;p class="prompt"&gt;evil spirit&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is a demon ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="121" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" ht="56" hidden="1">
       <c r="A121">
         <f>ROW()</f>
         <v>121</v>
@@ -5713,7 +5717,7 @@
         <v>&lt;div class="clue jbg" rel="#121"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="121"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is solitary ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="122" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" ht="56" hidden="1">
       <c r="A122">
         <f>ROW()</f>
         <v>122</v>
@@ -5729,7 +5733,7 @@
         <v>&lt;div class="clue jbg" rel="#122"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="122"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is possesed ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="123" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" ht="56" hidden="1">
       <c r="A123">
         <f>ROW()</f>
         <v>123</v>
@@ -5745,7 +5749,7 @@
         <v>&lt;div class="clue jbg" rel="#123"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="123"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt;What is a stable ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="124" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" ht="56" hidden="1">
       <c r="A124">
         <f>ROW()</f>
         <v>124</v>
@@ -5755,7 +5759,7 @@
         <v>&lt;div class="clue jbg" rel="#124"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="124"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt; ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="125" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" ht="56" hidden="1">
       <c r="A125">
         <f>ROW()</f>
         <v>125</v>
@@ -5765,7 +5769,7 @@
         <v>&lt;div class="clue jbg" rel="#125"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="125"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt; ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="56" hidden="1">
       <c r="A126">
         <f>ROW()</f>
         <v>126</v>
@@ -5775,13 +5779,13 @@
         <v>&lt;div class="clue jbg" rel="#126"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id="126"&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt; ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="127" spans="1:9" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" ht="56" hidden="1">
       <c r="H127" s="3" t="str">
         <f t="shared" si="3"/>
         <v>&lt;div class="clue jbg" rel="#"&gt;&lt;h2 class="value"&gt;&lt;/h2&gt; &lt;/div&gt;&lt;div class="apple_overlay" id=""&gt; &lt;p class="prompt"&gt;&lt;/p&gt;&lt;div class="slider"&gt;&lt;span class="button"&gt;Reveal Answer&lt;/span&gt;&lt;p class="response"&gt; ( )&lt;/p&gt;&lt;/div&gt;&lt;/div&gt;</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="84">
       <c r="A128">
         <f>ROW()</f>
         <v>128</v>
@@ -5812,7 +5816,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="129" spans="1:9" ht="90" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" ht="70">
       <c r="A129">
         <f>ROW()</f>
         <v>129</v>
@@ -5855,7 +5859,12 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5867,16 +5876,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="A1" s="8" t="s">
         <v>197</v>
       </c>
@@ -5887,7 +5896,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" s="9" t="s">
         <v>54</v>
       </c>
@@ -5898,7 +5907,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" s="9" t="s">
         <v>49</v>
       </c>
@@ -5909,7 +5918,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" s="9" t="s">
         <v>10</v>
       </c>
@@ -5920,7 +5929,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" s="9" t="s">
         <v>31</v>
       </c>
@@ -5931,7 +5940,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" s="9" t="s">
         <v>7</v>
       </c>
@@ -5942,7 +5951,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" s="9" t="s">
         <v>12</v>
       </c>
@@ -5953,14 +5962,14 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="9" t="s">
         <v>198</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="9" t="s">
         <v>199</v>
       </c>
@@ -5973,6 +5982,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5982,8 +5996,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>